<commit_message>
add work with nartis
</commit_message>
<xml_diff>
--- a/prizmer/static/excel/electric_template_for_load.xlsx
+++ b/prizmer/static/excel/electric_template_for_load.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Electr_k1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Electr_k1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="52">
   <si>
     <t xml:space="preserve">Населенный пункт</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t xml:space="preserve">4* При прогрузке приборов, которые будут опрашиваться через UM-RTU1 в колонке F необходимо ввести id в рамках УМ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ВРУ АВР</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нартис СПОДЭС</t>
   </si>
   <si>
     <t xml:space="preserve">5* Если необходимо чтение из прибора реактивной энергии R+ и/или Получасовых профилей мощности A+ и R+ (обязательно для отчёта по форме 80020), то поставьте в соответсвующей колонке "+". Если чтение этих параметров не нужно (НЕ рекомендуется для квартир), то оставьте это поле пустым или напишите "-"</t>
@@ -347,11 +353,15 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -364,15 +374,15 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -384,31 +394,31 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -416,39 +426,39 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -556,520 +566,662 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+      <selection pane="topLeft" activeCell="K28" activeCellId="0" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="6.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="9.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="72.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11" t="n">
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12" t="n">
         <v>28376066</v>
       </c>
-      <c r="H2" s="11" t="n">
+      <c r="H2" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="12" t="n">
+      <c r="J2" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="13" t="n">
+      <c r="L2" s="14" t="n">
         <v>4003</v>
       </c>
-      <c r="M2" s="14"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
     </row>
     <row r="3" customFormat="false" ht="12.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="11" t="n">
+      <c r="E3" s="10"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12" t="n">
         <v>38136243</v>
       </c>
-      <c r="H3" s="11" t="n">
+      <c r="H3" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="12" t="n">
+      <c r="J3" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="13" t="n">
+      <c r="L3" s="14" t="n">
         <v>4003</v>
       </c>
-      <c r="M3" s="14"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
     </row>
     <row r="4" customFormat="false" ht="12.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="11" t="n">
+      <c r="E4" s="17"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="12" t="n">
         <v>29936803</v>
       </c>
-      <c r="H4" s="9" t="n">
+      <c r="H4" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="17" t="n">
+      <c r="J4" s="18" t="n">
         <v>80</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="13" t="n">
+      <c r="L4" s="14" t="n">
         <v>5004</v>
       </c>
-      <c r="M4" s="14"/>
-      <c r="N4" s="15" t="s">
+      <c r="M4" s="15"/>
+      <c r="N4" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="15" t="s">
+      <c r="O4" s="16" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="11" t="n">
+      <c r="E5" s="11"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="12" t="n">
         <v>29936836</v>
       </c>
-      <c r="H5" s="9" t="n">
+      <c r="H5" s="10" t="n">
         <v>14</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="17" t="n">
+      <c r="J5" s="18" t="n">
         <v>80</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="13" t="n">
+      <c r="L5" s="14" t="n">
         <v>5004</v>
       </c>
-      <c r="M5" s="14"/>
-      <c r="N5" s="15" t="s">
+      <c r="M5" s="15"/>
+      <c r="N5" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="15" t="s">
+      <c r="O5" s="16" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="11" t="n">
+      <c r="E6" s="11"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="12" t="n">
         <v>29937023</v>
       </c>
-      <c r="H6" s="9" t="n">
+      <c r="H6" s="10" t="n">
         <v>15</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="10" t="n">
+      <c r="J6" s="11" t="n">
         <v>30</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="13" t="n">
+      <c r="L6" s="14" t="n">
         <v>5004</v>
       </c>
-      <c r="M6" s="14"/>
-      <c r="N6" s="15" t="s">
+      <c r="M6" s="15"/>
+      <c r="N6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="16" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="11" t="n">
+      <c r="E7" s="11"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="12" t="n">
         <v>31571813</v>
       </c>
-      <c r="H7" s="9" t="n">
+      <c r="H7" s="10" t="n">
         <v>16</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="10" t="n">
+      <c r="J7" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="13" t="n">
+      <c r="L7" s="14" t="n">
         <v>5004</v>
       </c>
-      <c r="M7" s="14"/>
-      <c r="N7" s="15" t="s">
+      <c r="M7" s="15"/>
+      <c r="N7" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="O7" s="15" t="s">
+      <c r="O7" s="16" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="19" t="n">
+      <c r="E8" s="15"/>
+      <c r="F8" s="20" t="n">
         <v>701</v>
       </c>
-      <c r="G8" s="20" t="n">
+      <c r="G8" s="21" t="n">
         <v>32375394</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="18" t="n">
+      <c r="J8" s="19" t="n">
         <v>80</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="K8" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="23" t="n">
+      <c r="L8" s="24" t="n">
         <v>4002</v>
       </c>
-      <c r="M8" s="14"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="Q8" s="24" t="s">
+      <c r="M8" s="15"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="Q8" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="24"/>
-      <c r="U8" s="24"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="24"/>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="24"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="25"/>
+      <c r="V8" s="25"/>
+      <c r="W8" s="25"/>
+      <c r="X8" s="25"/>
+      <c r="Y8" s="25"/>
+      <c r="Z8" s="25"/>
     </row>
     <row r="9" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="19" t="n">
+      <c r="E9" s="15"/>
+      <c r="F9" s="20" t="n">
         <v>702</v>
       </c>
-      <c r="G9" s="20" t="n">
+      <c r="G9" s="21" t="n">
         <v>32952201</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="18" t="n">
+      <c r="J9" s="19" t="n">
         <v>80</v>
       </c>
-      <c r="K9" s="22" t="s">
+      <c r="K9" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="L9" s="23" t="n">
+      <c r="L9" s="24" t="n">
         <v>4002</v>
       </c>
-      <c r="M9" s="14"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="Q9" s="24" t="s">
+      <c r="M9" s="15"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="Q9" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
-      <c r="T9" s="24"/>
-      <c r="U9" s="24"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="24"/>
-      <c r="X9" s="24"/>
-      <c r="Y9" s="24"/>
-      <c r="Z9" s="24"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="25"/>
+      <c r="W9" s="25"/>
+      <c r="X9" s="25"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25"/>
     </row>
     <row r="10" customFormat="false" ht="26.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>7520107</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="25" t="s">
+      <c r="I10" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="J10" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K10" s="22" t="s">
+      <c r="K10" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="L10" s="23" t="n">
+      <c r="L10" s="24" t="n">
         <v>4002</v>
       </c>
-      <c r="Q10" s="24" t="s">
+      <c r="Q10" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="R10" s="24"/>
-      <c r="S10" s="24"/>
-      <c r="T10" s="24"/>
-      <c r="U10" s="24"/>
-      <c r="V10" s="24"/>
-      <c r="W10" s="24"/>
-      <c r="X10" s="24"/>
-      <c r="Y10" s="24"/>
-      <c r="Z10" s="24"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="25"/>
+      <c r="W10" s="25"/>
+      <c r="X10" s="25"/>
+      <c r="Y10" s="25"/>
+      <c r="Z10" s="25"/>
     </row>
     <row r="11" customFormat="false" ht="24.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="25" t="n">
+      <c r="G11" s="26" t="n">
         <v>127205047</v>
       </c>
-      <c r="H11" s="25" t="n">
+      <c r="H11" s="26" t="n">
         <v>127205047</v>
       </c>
-      <c r="I11" s="25" t="s">
+      <c r="I11" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="J11" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K11" s="22" t="s">
+      <c r="K11" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="L11" s="23" t="n">
+      <c r="L11" s="24" t="n">
         <v>4002</v>
       </c>
-      <c r="Q11" s="24" t="s">
+      <c r="Q11" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="24"/>
-      <c r="U11" s="24"/>
-      <c r="V11" s="24"/>
-      <c r="W11" s="24"/>
-      <c r="X11" s="24"/>
-      <c r="Y11" s="24"/>
-      <c r="Z11" s="24"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="25"/>
+      <c r="U11" s="25"/>
+      <c r="V11" s="25"/>
+      <c r="W11" s="25"/>
+      <c r="X11" s="25"/>
+      <c r="Y11" s="25"/>
+      <c r="Z11" s="25"/>
     </row>
     <row r="12" customFormat="false" ht="38.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="Q12" s="24" t="s">
+      <c r="A12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="24"/>
-      <c r="U12" s="24"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="24"/>
-      <c r="X12" s="24"/>
-      <c r="Y12" s="24"/>
-      <c r="Z12" s="24"/>
+      <c r="G12" s="26" t="n">
+        <v>127205047</v>
+      </c>
+      <c r="H12" s="26" t="n">
+        <v>19</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="L12" s="24" t="n">
+        <v>4002</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q12" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+      <c r="T12" s="25"/>
+      <c r="U12" s="25"/>
+      <c r="V12" s="25"/>
+      <c r="W12" s="25"/>
+      <c r="X12" s="25"/>
+      <c r="Y12" s="25"/>
+      <c r="Z12" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1081,16 +1233,14 @@
   </mergeCells>
   <conditionalFormatting sqref="G8:G9">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G8:G9">
     <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D11">
+  <conditionalFormatting sqref="D8:D12">
     <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>